<commit_message>
second part complete using external file
</commit_message>
<xml_diff>
--- a/src/excelFiles/players.xlsx
+++ b/src/excelFiles/players.xlsx
@@ -4,24 +4,37 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="10515" windowHeight="4695"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15060" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="Players" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>llano.marco@gmail.com</t>
   </si>
   <si>
     <t>Team Member</t>
+  </si>
+  <si>
+    <t>marcollano5@hotmail.com</t>
+  </si>
+  <si>
+    <t>Scum Master</t>
+  </si>
+  <si>
+    <t>marco_llano5@hotmail.com</t>
+  </si>
+  <si>
+    <t>Product Owner</t>
   </si>
 </sst>
 </file>
@@ -66,10 +79,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -372,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -388,9 +402,27 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>